<commit_message>
Test cases added into Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66CC93F-DA15-414A-A948-35D3067C50C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8F53CE-4A75-465E-B18D-65485FFC3C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" activeTab="4" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="TC_01_AddEmployee" sheetId="2" r:id="rId2"/>
-    <sheet name="TC_02_AddUser" sheetId="3" r:id="rId3"/>
+    <sheet name="TC_03_EditEmployee" sheetId="4" r:id="rId3"/>
+    <sheet name="TC_04_ApplyLeave" sheetId="5" r:id="rId4"/>
+    <sheet name="TC_05_RecruitmentCandidate" sheetId="6" r:id="rId5"/>
+    <sheet name="TC_02_AddUser" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="145">
   <si>
     <t>S. No</t>
   </si>
@@ -305,6 +308,171 @@
   </si>
   <si>
     <t>AddUser_ConfirmPassword</t>
+  </si>
+  <si>
+    <t>EditEmployee</t>
+  </si>
+  <si>
+    <t>TC_03_01</t>
+  </si>
+  <si>
+    <t>TC_03-02</t>
+  </si>
+  <si>
+    <t>TC_03_03</t>
+  </si>
+  <si>
+    <t>TC_03_04</t>
+  </si>
+  <si>
+    <t>TC_03_05</t>
+  </si>
+  <si>
+    <t>This test case will be Editing Employee into the Orange HRM</t>
+  </si>
+  <si>
+    <t>TC_04_01</t>
+  </si>
+  <si>
+    <t>TC_04_02</t>
+  </si>
+  <si>
+    <t>TC_04_03</t>
+  </si>
+  <si>
+    <t>TC_04_04</t>
+  </si>
+  <si>
+    <t>TC_04_05</t>
+  </si>
+  <si>
+    <t>ApplyLeave</t>
+  </si>
+  <si>
+    <t>This test case will Apply leave in the Orange HRM</t>
+  </si>
+  <si>
+    <t>TC_05_01</t>
+  </si>
+  <si>
+    <t>TC_05_02</t>
+  </si>
+  <si>
+    <t>TC_05_03</t>
+  </si>
+  <si>
+    <t>TC_05_04</t>
+  </si>
+  <si>
+    <t>TC_05_05</t>
+  </si>
+  <si>
+    <t>RecruitmentCandidate</t>
+  </si>
+  <si>
+    <t>This test case will be Recruiting Candidate in the Orange HRM</t>
+  </si>
+  <si>
+    <t>TC_06_01</t>
+  </si>
+  <si>
+    <t>TC_06_02</t>
+  </si>
+  <si>
+    <t>TC_06_03</t>
+  </si>
+  <si>
+    <t>TC_06_04</t>
+  </si>
+  <si>
+    <t>TC_06_05</t>
+  </si>
+  <si>
+    <t>TC_07_01</t>
+  </si>
+  <si>
+    <t>TC_07_02</t>
+  </si>
+  <si>
+    <t>TC_07_03</t>
+  </si>
+  <si>
+    <t>TC_07_04</t>
+  </si>
+  <si>
+    <t>TC_07_05</t>
+  </si>
+  <si>
+    <t>TC_08_01</t>
+  </si>
+  <si>
+    <t>TC_08_02</t>
+  </si>
+  <si>
+    <t>TC_08_03</t>
+  </si>
+  <si>
+    <t>TC_08_04</t>
+  </si>
+  <si>
+    <t>PurchaseCOD</t>
+  </si>
+  <si>
+    <t>ReOrder</t>
+  </si>
+  <si>
+    <t>AllOrderTotal</t>
+  </si>
+  <si>
+    <t>This test case will be PurchaseCOD on DemoWebShop</t>
+  </si>
+  <si>
+    <t>This test case will be Reorder on DemoWebShop</t>
+  </si>
+  <si>
+    <t>This test case will be All orders total in DemoWebShop</t>
+  </si>
+  <si>
+    <t>Edit Employee</t>
+  </si>
+  <si>
+    <t>NewLastName</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>EventInformation</t>
+  </si>
+  <si>
+    <t>LeaveType</t>
+  </si>
+  <si>
+    <t>LeaveFromDate</t>
+  </si>
+  <si>
+    <t>LeaveToDate</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>LinkedInURL</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>RecruitmentStage</t>
   </si>
 </sst>
 </file>
@@ -692,18 +860,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113BCE2C-B803-46ED-B963-DE246F732555}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -743,7 +913,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -760,7 +930,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -777,7 +947,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -794,7 +964,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -811,7 +981,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -828,7 +998,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -845,7 +1015,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -862,7 +1032,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -879,7 +1049,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -896,233 +1066,494 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
       <c r="F12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
       <c r="F13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
       <c r="F14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
       <c r="F15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
       <c r="F16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
       <c r="F17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
       <c r="F18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
       <c r="F19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
       <c r="F20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
       <c r="F21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
+        <v>110</v>
+      </c>
       <c r="F22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>110</v>
+      </c>
       <c r="F23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>110</v>
+      </c>
       <c r="F24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
       <c r="F25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" t="s">
+        <v>110</v>
+      </c>
       <c r="F26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
       <c r="F27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
       <c r="F28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
       <c r="F29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
       <c r="F30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
       <c r="F31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s">
+        <v>129</v>
+      </c>
       <c r="F32" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
+        <v>129</v>
+      </c>
       <c r="F33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>129</v>
+      </c>
       <c r="F34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" t="s">
+        <v>129</v>
+      </c>
       <c r="F35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" t="s">
+        <v>129</v>
+      </c>
       <c r="F36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" t="s">
+        <v>130</v>
+      </c>
       <c r="F37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s">
+        <v>130</v>
+      </c>
       <c r="F38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
       <c r="F39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" t="s">
+        <v>130</v>
       </c>
       <c r="F40" t="s">
         <v>54</v>
@@ -1140,23 +1571,23 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1229,7 +1660,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1692,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1724,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1756,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1371,26 +1802,500 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BC94E3-296F-4311-83A2-9D6323C2EB33}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B1B19367-98D1-4B82-8356-A257C784E807}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B9FCF534-0EEF-43DA-8FFE-A72C5C3C3EFF}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B6762509-80AD-4CF1-9F99-84AC5E35F57C}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{28DE3539-5410-4447-918C-6DD46CC59ABE}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{E5813CFD-8EB7-4723-B9D3-B32316710701}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C415BAA9-6369-4BAB-B424-B445438157B3}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D7788139-C4A5-4FCD-8C7F-3FF6153B2B78}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{3E13B705-B6A7-41A9-87E5-AA5D3FDFBA6E}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{0A7EA8E3-7EFB-46C4-9871-473A77BA051C}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{2AF26926-5989-4147-A1F6-28D262924D65}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{1E2DEF20-B73B-4528-A2E8-BB36839585C6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B1A084F-7AA5-4755-AE91-33EB517F2ADC}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{CFE7350B-178E-4DA4-875A-E0C0271D03FC}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{8D9770EB-54B7-4AFD-8862-394630BD7DD7}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{719AFC6C-6EAC-43F2-9DB8-BD0738976F89}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{63176F78-05F6-4B70-AE9D-B7C1B72D41E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F6A3B6-0769-41C7-9100-21709CD78AE4}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +2324,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1442,7 +2347,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +2370,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1488,7 +2393,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +2416,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Random generation and testdata is added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8F53CE-4A75-465E-B18D-65485FFC3C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ABC52A-D074-4A62-8467-1BBE02D0B8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" activeTab="4" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" activeTab="5" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
-    <sheet name="TC_01_AddEmployee" sheetId="2" r:id="rId2"/>
-    <sheet name="TC_03_EditEmployee" sheetId="4" r:id="rId3"/>
-    <sheet name="TC_04_ApplyLeave" sheetId="5" r:id="rId4"/>
-    <sheet name="TC_05_RecruitmentCandidate" sheetId="6" r:id="rId5"/>
-    <sheet name="TC_02_AddUser" sheetId="3" r:id="rId6"/>
+    <sheet name="AddEmployee" sheetId="2" r:id="rId2"/>
+    <sheet name="AddUser" sheetId="3" r:id="rId3"/>
+    <sheet name="EditEmployee" sheetId="4" r:id="rId4"/>
+    <sheet name="ApplyLeave" sheetId="5" r:id="rId5"/>
+    <sheet name="RecruitmentCandidate" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="174">
   <si>
     <t>S. No</t>
   </si>
@@ -439,15 +439,9 @@
     <t>NewLastName</t>
   </si>
   <si>
-    <t>MaritalStatus</t>
-  </si>
-  <si>
     <t>Nationality</t>
   </si>
   <si>
-    <t>EventInformation</t>
-  </si>
-  <si>
     <t>LeaveType</t>
   </si>
   <si>
@@ -473,6 +467,99 @@
   </si>
   <si>
     <t>RecruitmentStage</t>
+  </si>
+  <si>
+    <t>TC_03_02</t>
+  </si>
+  <si>
+    <t>Australian</t>
+  </si>
+  <si>
+    <t>Canadian</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Contract Renewal</t>
+  </si>
+  <si>
+    <t>Cost Center Move</t>
+  </si>
+  <si>
+    <t>EEO Job Category Changed</t>
+  </si>
+  <si>
+    <t>First Time Addition</t>
+  </si>
+  <si>
+    <t>FLSA Exemption Changed</t>
+  </si>
+  <si>
+    <t>Living Allowance</t>
+  </si>
+  <si>
+    <t>9000.00</t>
+  </si>
+  <si>
+    <t>12500.00</t>
+  </si>
+  <si>
+    <t>15000.00</t>
+  </si>
+  <si>
+    <t>25000.00</t>
+  </si>
+  <si>
+    <t>45000.00</t>
+  </si>
+  <si>
+    <t>EPF</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Promoted</t>
+  </si>
+  <si>
+    <t>Initial Contract</t>
+  </si>
+  <si>
+    <t>Joined</t>
+  </si>
+  <si>
+    <t>EEO Pay Band Changed</t>
+  </si>
+  <si>
+    <t>Job_EventInformation</t>
+  </si>
+  <si>
+    <t>Salary_EventInformation</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>9632589630</t>
+  </si>
+  <si>
+    <t>6589145231</t>
+  </si>
+  <si>
+    <t>8521474560</t>
+  </si>
+  <si>
+    <t>7569842103</t>
+  </si>
+  <si>
+    <t>8596485213</t>
   </si>
 </sst>
 </file>
@@ -537,12 +624,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -860,20 +948,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113BCE2C-B803-46ED-B963-DE246F732555}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="62.109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -913,7 +1001,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -930,7 +1018,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -947,7 +1035,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -964,7 +1052,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -981,7 +1069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -998,7 +1086,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1032,7 +1120,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1066,7 +1154,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1083,7 +1171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1100,7 +1188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1205,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1134,7 +1222,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1239,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1168,7 +1256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1185,7 +1273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1202,7 +1290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1219,7 +1307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1253,7 +1341,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1270,7 +1358,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1287,7 +1375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1304,7 +1392,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1321,7 +1409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1355,7 +1443,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1372,7 +1460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1389,7 +1477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1406,7 +1494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1423,7 +1511,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1440,7 +1528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1457,7 +1545,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1474,7 +1562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1491,7 +1579,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1508,7 +1596,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1542,7 +1630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1571,23 +1659,23 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1716,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1660,7 +1748,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1780,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1724,7 +1812,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1756,7 +1844,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1802,500 +1890,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BC94E3-296F-4311-83A2-9D6323C2EB33}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="6.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{B1B19367-98D1-4B82-8356-A257C784E807}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{B9FCF534-0EEF-43DA-8FFE-A72C5C3C3EFF}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{B6762509-80AD-4CF1-9F99-84AC5E35F57C}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{28DE3539-5410-4447-918C-6DD46CC59ABE}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{E5813CFD-8EB7-4723-B9D3-B32316710701}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C415BAA9-6369-4BAB-B424-B445438157B3}">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{D7788139-C4A5-4FCD-8C7F-3FF6153B2B78}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{3E13B705-B6A7-41A9-87E5-AA5D3FDFBA6E}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{0A7EA8E3-7EFB-46C4-9871-473A77BA051C}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{2AF26926-5989-4147-A1F6-28D262924D65}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{1E2DEF20-B73B-4528-A2E8-BB36839585C6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
-  <dimension ref="A1:K15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="6.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B1A084F-7AA5-4755-AE91-33EB517F2ADC}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{CFE7350B-178E-4DA4-875A-E0C0271D03FC}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{8D9770EB-54B7-4AFD-8862-394630BD7DD7}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{719AFC6C-6EAC-43F2-9DB8-BD0738976F89}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{63176F78-05F6-4B70-AE9D-B7C1B72D41E3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F6A3B6-0769-41C7-9100-21709CD78AE4}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +1938,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2347,7 +1961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2370,7 +1984,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2393,7 +2007,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2416,7 +2030,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2459,4 +2073,604 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BC94E3-296F-4311-83A2-9D6323C2EB33}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="H2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="H3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="H5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>164</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="H6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M6" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B1B19367-98D1-4B82-8356-A257C784E807}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B9FCF534-0EEF-43DA-8FFE-A72C5C3C3EFF}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B6762509-80AD-4CF1-9F99-84AC5E35F57C}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{28DE3539-5410-4447-918C-6DD46CC59ABE}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{E5813CFD-8EB7-4723-B9D3-B32316710701}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C415BAA9-6369-4BAB-B424-B445438157B3}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D7788139-C4A5-4FCD-8C7F-3FF6153B2B78}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{3E13B705-B6A7-41A9-87E5-AA5D3FDFBA6E}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{0A7EA8E3-7EFB-46C4-9871-473A77BA051C}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{2AF26926-5989-4147-A1F6-28D262924D65}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{1E2DEF20-B73B-4528-A2E8-BB36839585C6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B1A084F-7AA5-4755-AE91-33EB517F2ADC}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{CFE7350B-178E-4DA4-875A-E0C0271D03FC}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{8D9770EB-54B7-4AFD-8862-394630BD7DD7}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{719AFC6C-6EAC-43F2-9DB8-BD0738976F89}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{63176F78-05F6-4B70-AE9D-B7C1B72D41E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in Excel file and Added random functtions
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ABC52A-D074-4A62-8467-1BBE02D0B8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75133031-7C1C-45A4-BF77-4E4E8ED2F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" activeTab="5" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="EditEmployee" sheetId="4" r:id="rId4"/>
     <sheet name="ApplyLeave" sheetId="5" r:id="rId5"/>
     <sheet name="RecruitmentCandidate" sheetId="6" r:id="rId6"/>
+    <sheet name="PurchaseCOD" sheetId="7" r:id="rId7"/>
+    <sheet name="ReOrderCOD" sheetId="8" r:id="rId8"/>
+    <sheet name="AllOrdersTotal" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="200">
   <si>
     <t>S. No</t>
   </si>
@@ -457,9 +460,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>LinkedInURL</t>
   </si>
   <si>
@@ -560,6 +560,87 @@
   </si>
   <si>
     <t>8596485213</t>
+  </si>
+  <si>
+    <t>Adduser_password</t>
+  </si>
+  <si>
+    <t>FMLA - US</t>
+  </si>
+  <si>
+    <t>Maternity Leave - US</t>
+  </si>
+  <si>
+    <t>Sick Leave - US</t>
+  </si>
+  <si>
+    <t>Work From Home - US</t>
+  </si>
+  <si>
+    <t>11-August-2022</t>
+  </si>
+  <si>
+    <t>11-June-2022</t>
+  </si>
+  <si>
+    <t>11-July-2022</t>
+  </si>
+  <si>
+    <t>15-June-2022</t>
+  </si>
+  <si>
+    <t>15-July-2022</t>
+  </si>
+  <si>
+    <t>15-September-2022</t>
+  </si>
+  <si>
+    <t>1-October-2022</t>
+  </si>
+  <si>
+    <t>11-October-2022</t>
+  </si>
+  <si>
+    <t>1-July-2022</t>
+  </si>
+  <si>
+    <t>Credit Analyst</t>
+  </si>
+  <si>
+    <t>Software QA Engineer</t>
+  </si>
+  <si>
+    <t>DevOps Engineer</t>
+  </si>
+  <si>
+    <t>Sales Manager</t>
+  </si>
+  <si>
+    <t>Shortlisted</t>
+  </si>
+  <si>
+    <t>StageChanges</t>
+  </si>
+  <si>
+    <t>Hired</t>
+  </si>
+  <si>
+    <t>aarosagarch@gmail.com</t>
+  </si>
+  <si>
+    <t>LoginEmail</t>
+  </si>
+  <si>
+    <t>ReOrderCOD</t>
+  </si>
+  <si>
+    <t>AllOrdersTotal</t>
+  </si>
+  <si>
+    <t>TC_08_05</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -946,22 +1027,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113BCE2C-B803-46ED-B963-DE246F732555}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="62.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="62.08984375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +1065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1001,7 +1082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1018,7 +1099,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1069,7 +1150,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,7 +1184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1201,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1218,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1154,7 +1235,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1171,7 +1252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1188,7 +1269,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1205,7 +1286,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1222,7 +1303,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1239,7 +1320,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1256,7 +1337,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1273,7 +1354,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1290,7 +1371,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1307,7 +1388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1324,7 +1405,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1358,7 +1439,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1375,7 +1456,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1392,7 +1473,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1409,7 +1490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1426,7 +1507,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1443,7 +1524,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1460,7 +1541,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1477,7 +1558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1494,7 +1575,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1511,7 +1592,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1528,7 +1609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1545,7 +1626,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1562,7 +1643,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1660,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1613,7 +1694,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1630,7 +1711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1644,6 +1725,23 @@
         <v>130</v>
       </c>
       <c r="F40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" t="s">
+        <v>198</v>
+      </c>
+      <c r="C41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1659,23 +1757,24 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1815,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1748,7 +1847,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1780,7 +1879,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1812,7 +1911,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1943,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1891,25 +1990,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F6A3B6-0769-41C7-9100-21709CD78AE4}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.90625" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1937,8 +2038,14 @@
       <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1960,8 +2067,11 @@
       <c r="I2" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1983,8 +2093,11 @@
       <c r="I3" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2006,8 +2119,11 @@
       <c r="I4" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2029,8 +2145,11 @@
       <c r="I5" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2050,6 +2169,9 @@
         <v>72</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2070,6 +2192,11 @@
     <hyperlink ref="I4" r:id="rId13" xr:uid="{7A88AAA5-59F4-409D-9B87-BA2E23E1DB96}"/>
     <hyperlink ref="I5" r:id="rId14" xr:uid="{B4EE66FD-9B41-4451-9AD1-6CFB4EF1B70E}"/>
     <hyperlink ref="I6" r:id="rId15" xr:uid="{9A236127-DDFA-4E2E-B98B-C45C011D8467}"/>
+    <hyperlink ref="K2" r:id="rId16" xr:uid="{9435A09B-03C4-456F-AB02-BD1DF82A3314}"/>
+    <hyperlink ref="K3" r:id="rId17" xr:uid="{068D1552-2FDF-4461-828C-9E7C26A732F1}"/>
+    <hyperlink ref="K4" r:id="rId18" xr:uid="{CDD9A8EA-2A48-4B13-BA61-0E14F7ADDC7D}"/>
+    <hyperlink ref="K5" r:id="rId19" xr:uid="{E4E615BB-764A-4931-9E86-BEE62D6ADD01}"/>
+    <hyperlink ref="K6" r:id="rId20" xr:uid="{0556187D-DF27-4001-9D52-7B4E3050E6E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2083,23 +2210,23 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2128,22 +2255,22 @@
         <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2161,33 +2288,33 @@
       </c>
       <c r="F2" s="3"/>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2" t="s">
         <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
         <v>131</v>
@@ -2200,28 +2327,28 @@
       </c>
       <c r="F3" s="3"/>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I3" t="s">
         <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="M3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2239,28 +2366,28 @@
       </c>
       <c r="F4" s="3"/>
       <c r="H4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I4" t="s">
         <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2278,28 +2405,28 @@
       </c>
       <c r="F5" s="3"/>
       <c r="H5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" t="s">
         <v>76</v>
       </c>
       <c r="J5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2317,25 +2444,25 @@
       </c>
       <c r="F6" s="3"/>
       <c r="H6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I6" t="s">
         <v>77</v>
       </c>
       <c r="J6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2356,21 +2483,21 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2396,12 +2523,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>102</v>
@@ -2412,13 +2539,22 @@
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>102</v>
@@ -2429,13 +2565,22 @@
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
         <v>102</v>
@@ -2446,13 +2591,22 @@
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>102</v>
@@ -2463,13 +2617,22 @@
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>102</v>
@@ -2479,6 +2642,15 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2490,6 +2662,7 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{1E2DEF20-B73B-4528-A2E8-BB36839585C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2497,25 +2670,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2547,15 +2721,15 @@
         <v>141</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>109</v>
@@ -2566,13 +2740,22 @@
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>109</v>
@@ -2583,13 +2766,22 @@
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>109</v>
@@ -2600,13 +2792,22 @@
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>109</v>
@@ -2617,13 +2818,22 @@
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>109</v>
@@ -2634,32 +2844,41 @@
       <c r="E6" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -2673,4 +2892,412 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1433F4D-AA94-4C23-B8F4-C641A3F219D9}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{5E9C8625-D106-45AE-A2F9-5E51D61CBFE0}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{38558A90-7C00-4866-976E-FA2E288CA368}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4B9CF97E-D29B-4384-9EAE-4F78571429B9}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{A3236F57-96B7-4DD8-9320-11644DBC8202}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{131E80A2-E254-4E79-8641-D5C01CA5B12F}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{613FBB1A-D0E5-4250-91B2-D8877C5F6264}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{D7E951F1-1C70-4772-BC07-8583BC8EB499}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{718D9A1F-4054-48EA-A9CE-61C4537D8E96}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{81E76611-A800-4E21-91CC-AF4CF9543FA2}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{C444CDD7-BB16-419E-B5C5-21358CC413F1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A32D993-D624-4A5F-A345-C2B190736A2C}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DE886733-9328-4598-8D26-E2E719BAA614}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{3019D316-FB37-43DB-87A7-33E18FB5CD82}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{90CF8BD9-4299-4D2C-A6E1-C02B2C4151A3}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{32AFD8AC-0D8A-41C5-AD09-AD802DFB8225}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{AA10C6E8-1316-4338-9BD2-2A46560FE2B2}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{501950A3-5084-4882-858B-E6BAFABADEDB}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{FE589201-A794-4794-900A-88BEB315E8B2}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{743F8B8D-ABBD-4EA1-966E-0C897664994E}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{765635CE-6869-487C-9211-657684933A1F}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{91941414-F121-4A40-8824-143E9AA10739}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4CA563-4911-400A-8354-9E2AF7E9F3EA}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{120A6782-FC14-4FBD-848C-F97853D6EA15}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B311BEF8-42DB-45E5-9A9D-1BCB25F13E19}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{E4CE0763-8A28-4416-9741-714BE98D0BB9}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D1F49D72-4D38-4A68-BBDF-8B94B69A7A54}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{6B509648-60AA-4075-B57D-27717A8C17B5}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{245F1335-9C56-468E-A1AE-05869E1E5628}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{7B08F35D-70AF-484B-ABA0-080EAE0B48CC}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{A586EE84-37D0-43FD-8B5B-736945551CC0}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{A0358B6D-757E-4C6A-9987-E5335559A817}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{28272A4A-C9BF-4BFB-BFEF-F1A7FCCCD979}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Utilities are added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75133031-7C1C-45A4-BF77-4E4E8ED2F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6925930-036B-4549-B522-0B9A54A1C830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" activeTab="1" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="199">
   <si>
     <t>S. No</t>
   </si>
@@ -560,9 +560,6 @@
   </si>
   <si>
     <t>8596485213</t>
-  </si>
-  <si>
-    <t>Adduser_password</t>
   </si>
   <si>
     <t>FMLA - US</t>
@@ -1029,20 +1026,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113BCE2C-B803-46ED-B963-DE246F732555}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="62.109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1130,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1150,7 +1147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1167,7 +1164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1181,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1232,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1249,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1303,7 +1300,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1354,7 +1351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1388,7 +1385,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1402,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1456,7 +1453,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1473,7 +1470,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1490,7 +1487,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1541,7 +1538,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1558,7 +1555,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1575,7 +1572,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1592,7 +1589,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1609,7 +1606,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1626,7 +1623,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1643,7 +1640,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1660,7 +1657,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1677,7 +1674,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1694,7 +1691,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1711,7 +1708,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1728,12 +1725,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
         <v>127</v>
@@ -1756,25 +1753,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C14E7B3-7A94-4166-8B22-BEFE5B744D32}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1815,7 +1812,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1879,7 +1876,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1911,7 +1908,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1943,7 +1940,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1990,27 +1987,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F6A3B6-0769-41C7-9100-21709CD78AE4}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.90625" customWidth="1"/>
-    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2038,14 +2033,8 @@
       <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2067,11 +2056,8 @@
       <c r="I2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2093,11 +2079,8 @@
       <c r="I3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2119,11 +2102,8 @@
       <c r="I4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2145,11 +2125,8 @@
       <c r="I5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2169,9 +2146,6 @@
         <v>72</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2192,11 +2166,6 @@
     <hyperlink ref="I4" r:id="rId13" xr:uid="{7A88AAA5-59F4-409D-9B87-BA2E23E1DB96}"/>
     <hyperlink ref="I5" r:id="rId14" xr:uid="{B4EE66FD-9B41-4451-9AD1-6CFB4EF1B70E}"/>
     <hyperlink ref="I6" r:id="rId15" xr:uid="{9A236127-DDFA-4E2E-B98B-C45C011D8467}"/>
-    <hyperlink ref="K2" r:id="rId16" xr:uid="{9435A09B-03C4-456F-AB02-BD1DF82A3314}"/>
-    <hyperlink ref="K3" r:id="rId17" xr:uid="{068D1552-2FDF-4461-828C-9E7C26A732F1}"/>
-    <hyperlink ref="K4" r:id="rId18" xr:uid="{CDD9A8EA-2A48-4B13-BA61-0E14F7ADDC7D}"/>
-    <hyperlink ref="K5" r:id="rId19" xr:uid="{E4E615BB-764A-4931-9E86-BEE62D6ADD01}"/>
-    <hyperlink ref="K6" r:id="rId20" xr:uid="{0556187D-DF27-4001-9D52-7B4E3050E6E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2210,23 +2179,23 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2270,7 +2239,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2309,7 +2278,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2348,7 +2317,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2387,7 +2356,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2426,7 +2395,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2486,18 +2455,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2492,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2540,16 +2509,16 @@
         <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2566,16 +2535,16 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2592,16 +2561,16 @@
         <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2618,16 +2587,16 @@
         <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2644,13 +2613,13 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2674,22 +2643,22 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2721,10 +2690,10 @@
         <v>141</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2741,16 +2710,16 @@
         <v>72</v>
       </c>
       <c r="I2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J2" t="s">
         <v>190</v>
       </c>
-      <c r="J2" t="s">
-        <v>191</v>
-      </c>
       <c r="K2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2767,16 +2736,16 @@
         <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2793,16 +2762,16 @@
         <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2819,16 +2788,16 @@
         <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2845,40 +2814,40 @@
         <v>72</v>
       </c>
       <c r="I6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -2902,16 +2871,16 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2922,13 +2891,13 @@
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2939,13 +2908,13 @@
         <v>125</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2956,13 +2925,13 @@
         <v>125</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2973,13 +2942,13 @@
         <v>125</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2990,13 +2959,13 @@
         <v>125</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3007,7 +2976,7 @@
         <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
@@ -3038,16 +3007,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3058,13 +3027,13 @@
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3072,16 +3041,16 @@
         <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3089,16 +3058,16 @@
         <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3106,16 +3075,16 @@
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3123,16 +3092,16 @@
         <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3140,10 +3109,10 @@
         <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
@@ -3174,16 +3143,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3194,13 +3163,13 @@
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3208,16 +3177,16 @@
         <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3225,16 +3194,16 @@
         <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3242,16 +3211,16 @@
         <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3259,27 +3228,27 @@
         <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Excel Changes for AddEmployee
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6925930-036B-4549-B522-0B9A54A1C830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7EDF98-B665-45B5-856F-8E21A24BE300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" activeTab="1" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" activeTab="1" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="209">
   <si>
     <t>S. No</t>
   </si>
@@ -638,12 +638,43 @@
   </si>
   <si>
     <t>40</t>
+  </si>
+  <si>
+    <t>Winfred</t>
+  </si>
+  <si>
+    <t>Schimmel</t>
+  </si>
+  <si>
+    <t>05-06-1980</t>
+  </si>
+  <si>
+    <t>09-08-1995</t>
+  </si>
+  <si>
+    <t>12-10-1970</t>
+  </si>
+  <si>
+    <t>30-12-1999</t>
+  </si>
+  <si>
+    <t>31-05-2002</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>McLaughlin</t>
+  </si>
+  <si>
+    <t>0147</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -707,8 +738,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,16 +1061,16 @@
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="62.109375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.1796875"/>
+    <col min="3" max="3" customWidth="true" width="30.36328125"/>
+    <col min="4" max="4" customWidth="true" width="62.08984375"/>
+    <col min="5" max="5" customWidth="true" width="16.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1796875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1110,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1127,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1113,7 +1144,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1130,7 +1161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1178,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1164,7 +1195,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1212,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1198,7 +1229,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1215,7 +1246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1263,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1280,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1266,7 +1297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1283,7 +1314,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1300,7 +1331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1317,7 +1348,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1334,7 +1365,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1351,7 +1382,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1368,7 +1399,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1385,7 +1416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1402,7 +1433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1419,7 +1450,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1436,7 +1467,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1453,7 +1484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1470,7 +1501,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1487,7 +1518,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1504,7 +1535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1521,7 +1552,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1538,7 +1569,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1555,7 +1586,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1572,7 +1603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1620,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1606,7 +1637,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1623,7 +1654,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1640,7 +1671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1657,7 +1688,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1674,7 +1705,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1708,7 +1739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1725,7 +1756,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>198</v>
       </c>
@@ -1754,24 +1785,24 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36328125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.90625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.54296875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1843,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1831,8 +1862,8 @@
       <c r="H2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="4">
-        <v>29377</v>
+      <c r="I2" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="J2" t="s">
         <v>78</v>
@@ -1844,7 +1875,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1863,8 +1894,8 @@
       <c r="H3" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="4">
-        <v>34920</v>
+      <c r="I3" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="J3" t="s">
         <v>79</v>
@@ -1876,7 +1907,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1892,11 +1923,17 @@
       <c r="E4" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G4" t="s">
+        <v>207</v>
+      </c>
       <c r="H4" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="4">
-        <v>25853</v>
+      <c r="I4" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="J4" t="s">
         <v>80</v>
@@ -1907,8 +1944,11 @@
       <c r="L4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1927,8 +1967,8 @@
       <c r="H5" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="4">
-        <v>36524</v>
+      <c r="I5" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
@@ -1940,7 +1980,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1959,8 +1999,8 @@
       <c r="H6" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="4">
-        <v>37407</v>
+      <c r="I6" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
@@ -1993,19 +2033,19 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.08984375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.81640625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.54296875"/>
+    <col min="8" max="8" customWidth="true" width="23.90625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.08984375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2034,7 +2074,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2080,7 +2120,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2103,7 +2143,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2126,7 +2166,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2179,23 +2219,23 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.81640625"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="3" max="3" customWidth="true" width="15.6328125"/>
+    <col min="4" max="4" customWidth="true" width="11.81640625"/>
+    <col min="5" max="6" customWidth="true" width="15.1796875"/>
+    <col min="7" max="7" customWidth="true" width="13.36328125"/>
+    <col min="8" max="8" customWidth="true" width="10.90625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.54296875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6328125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.90625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,11 +2275,11 @@
       <c r="M1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2278,7 +2318,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2356,7 +2396,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2395,7 +2435,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2455,18 +2495,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.90625"/>
+    <col min="3" max="3" customWidth="true" width="19.0"/>
+    <col min="4" max="4" customWidth="true" width="11.6328125"/>
+    <col min="5" max="5" customWidth="true" width="12.81640625"/>
+    <col min="6" max="6" customWidth="true" width="20.90625"/>
+    <col min="7" max="7" customWidth="true" width="16.81640625"/>
+    <col min="8" max="8" customWidth="true" width="18.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2492,7 +2532,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2518,7 +2558,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2544,7 +2584,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2570,7 +2610,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2596,7 +2636,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2643,22 +2683,22 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.6328125"/>
+    <col min="2" max="2" customWidth="true" width="11.0"/>
+    <col min="3" max="3" customWidth="true" width="25.1796875"/>
+    <col min="4" max="4" customWidth="true" width="10.453125"/>
+    <col min="5" max="5" customWidth="true" width="14.54296875"/>
+    <col min="6" max="6" customWidth="true" width="11.1796875"/>
+    <col min="7" max="7" customWidth="true" width="10.453125"/>
+    <col min="8" max="8" customWidth="true" width="12.6328125"/>
+    <col min="9" max="9" customWidth="true" width="22.36328125"/>
+    <col min="10" max="10" customWidth="true" width="16.81640625"/>
+    <col min="11" max="11" customWidth="true" width="16.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2693,7 +2733,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2719,7 +2759,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2745,7 +2785,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2771,7 +2811,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2797,7 +2837,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2823,31 +2863,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -2871,16 +2911,16 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.90625"/>
+    <col min="2" max="2" customWidth="true" width="9.81640625"/>
+    <col min="3" max="3" customWidth="true" width="17.1796875"/>
+    <col min="4" max="4" customWidth="true" width="22.81640625"/>
+    <col min="5" max="5" customWidth="true" width="14.90625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2897,7 +2937,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2954,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2931,7 +2971,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2948,7 +2988,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2965,7 +3005,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3007,16 +3047,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="7.1796875"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375"/>
+    <col min="3" max="3" customWidth="true" width="22.81640625"/>
+    <col min="4" max="4" customWidth="true" width="25.1796875"/>
+    <col min="5" max="5" customWidth="true" width="16.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3033,7 +3073,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3050,7 +3090,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3067,7 +3107,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3084,7 +3124,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3141,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3143,16 +3183,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.81640625"/>
+    <col min="2" max="2" customWidth="true" width="12.0"/>
+    <col min="3" max="3" customWidth="true" width="16.08984375"/>
+    <col min="4" max="4" customWidth="true" width="23.90625"/>
+    <col min="5" max="5" customWidth="true" width="15.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3169,7 +3209,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3186,7 +3226,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3203,7 +3243,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3220,7 +3260,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3237,7 +3277,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Excel changes completed for Adduser testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="211">
   <si>
     <t>S. No</t>
   </si>
@@ -668,6 +668,12 @@
   </si>
   <si>
     <t>0147</t>
+  </si>
+  <si>
+    <t>1057</t>
+  </si>
+  <si>
+    <t>1059</t>
   </si>
 </sst>
 </file>
@@ -2027,7 +2033,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F6A3B6-0769-41C7-9100-21709CD78AE4}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
@@ -2164,6 +2170,9 @@
       </c>
       <c r="I5" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="M5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ExcelDAta Added to all TestCases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7EDF98-B665-45B5-856F-8E21A24BE300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7554164-0598-4021-A8CC-C0787231DA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" activeTab="1" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" firstSheet="2" activeTab="5" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="215">
   <si>
     <t>S. No</t>
   </si>
@@ -640,12 +640,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>Winfred</t>
-  </si>
-  <si>
-    <t>Schimmel</t>
-  </si>
-  <si>
     <t>05-06-1980</t>
   </si>
   <si>
@@ -670,17 +664,34 @@
     <t>0147</t>
   </si>
   <si>
-    <t>1057</t>
-  </si>
-  <si>
-    <t>1059</t>
+    <t>1079</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>sammie.wintheiser</t>
+  </si>
+  <si>
+    <t>0145</t>
+  </si>
+  <si>
+    <t>Bradtke</t>
+  </si>
+  <si>
+    <t>Layla</t>
+  </si>
+  <si>
+    <t>Haley</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ravi-c-1b35b1124/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1069,11 +1080,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.1796875"/>
-    <col min="3" max="3" customWidth="true" width="30.36328125"/>
-    <col min="4" max="4" customWidth="true" width="62.08984375"/>
-    <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1796875"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1790,22 +1801,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C14E7B3-7A94-4166-8B22-BEFE5B744D32}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.36328125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.90625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.54296875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
+    <col min="1" max="1" width="6.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -1869,7 +1881,7 @@
         <v>73</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J2" t="s">
         <v>78</v>
@@ -1901,7 +1913,7 @@
         <v>74</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J3" t="s">
         <v>79</v>
@@ -1930,16 +1942,16 @@
         <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H4" t="s">
         <v>75</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J4" t="s">
         <v>80</v>
@@ -1951,7 +1963,7 @@
         <v>85</v>
       </c>
       <c r="M4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -1974,7 +1986,7 @@
         <v>76</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J5" t="s">
         <v>78</v>
@@ -2006,7 +2018,7 @@
         <v>77</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J6" t="s">
         <v>79</v>
@@ -2041,17 +2053,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.08984375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.81640625"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.54296875"/>
-    <col min="8" max="8" customWidth="true" width="23.90625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="25.08984375"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.90625" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2138,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2149,7 +2161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2172,10 +2184,10 @@
         <v>72</v>
       </c>
       <c r="M5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2190,6 +2202,12 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" t="s">
+        <v>209</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>72</v>
@@ -2225,23 +2243,23 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.81640625"/>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="3" max="3" customWidth="true" width="15.6328125"/>
-    <col min="4" max="4" customWidth="true" width="11.81640625"/>
-    <col min="5" max="6" customWidth="true" width="15.1796875"/>
-    <col min="7" max="7" customWidth="true" width="13.36328125"/>
-    <col min="8" max="8" customWidth="true" width="10.90625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.54296875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6328125"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -2460,7 +2478,12 @@
       <c r="E6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G6" t="s">
+        <v>211</v>
+      </c>
       <c r="H6" t="s">
         <v>147</v>
       </c>
@@ -2501,18 +2524,18 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.90625"/>
-    <col min="3" max="3" customWidth="true" width="19.0"/>
-    <col min="4" max="4" customWidth="true" width="11.6328125"/>
-    <col min="5" max="5" customWidth="true" width="12.81640625"/>
-    <col min="6" max="6" customWidth="true" width="20.90625"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625"/>
-    <col min="8" max="8" customWidth="true" width="18.54296875"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2688,23 +2711,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.6328125"/>
-    <col min="2" max="2" customWidth="true" width="11.0"/>
-    <col min="3" max="3" customWidth="true" width="25.1796875"/>
-    <col min="4" max="4" customWidth="true" width="10.453125"/>
-    <col min="5" max="5" customWidth="true" width="14.54296875"/>
-    <col min="6" max="6" customWidth="true" width="11.1796875"/>
-    <col min="7" max="7" customWidth="true" width="10.453125"/>
-    <col min="8" max="8" customWidth="true" width="12.6328125"/>
-    <col min="9" max="9" customWidth="true" width="22.36328125"/>
-    <col min="10" max="10" customWidth="true" width="16.81640625"/>
-    <col min="11" max="11" customWidth="true" width="16.0"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="27.08984375" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2861,6 +2884,15 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" t="s">
+        <v>214</v>
       </c>
       <c r="I6" t="s">
         <v>186</v>
@@ -2917,16 +2949,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.90625"/>
-    <col min="2" max="2" customWidth="true" width="9.81640625"/>
-    <col min="3" max="3" customWidth="true" width="17.1796875"/>
-    <col min="4" max="4" customWidth="true" width="22.81640625"/>
-    <col min="5" max="5" customWidth="true" width="14.90625"/>
+    <col min="1" max="1" width="5.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3058,11 +3090,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.1796875"/>
-    <col min="2" max="2" customWidth="true" width="12.08984375"/>
-    <col min="3" max="3" customWidth="true" width="22.81640625"/>
-    <col min="4" max="4" customWidth="true" width="25.1796875"/>
-    <col min="5" max="5" customWidth="true" width="16.6328125"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3194,11 +3226,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.81640625"/>
-    <col min="2" max="2" customWidth="true" width="12.0"/>
-    <col min="3" max="3" customWidth="true" width="16.08984375"/>
-    <col min="4" max="4" customWidth="true" width="23.90625"/>
-    <col min="5" max="5" customWidth="true" width="15.54296875"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Parameterization is added for all testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7554164-0598-4021-A8CC-C0787231DA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F359A5C6-CC52-4F2E-848D-C9471FC3501D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" firstSheet="2" activeTab="5" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="235">
   <si>
     <t>S. No</t>
   </si>
@@ -673,12 +673,6 @@
     <t>sammie.wintheiser</t>
   </si>
   <si>
-    <t>0145</t>
-  </si>
-  <si>
-    <t>Bradtke</t>
-  </si>
-  <si>
     <t>Layla</t>
   </si>
   <si>
@@ -686,12 +680,79 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/ravi-c-1b35b1124/</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>McKenzie</t>
+  </si>
+  <si>
+    <t>1132</t>
+  </si>
+  <si>
+    <t>Wiza</t>
+  </si>
+  <si>
+    <t>Jayna</t>
+  </si>
+  <si>
+    <t>Cronin</t>
+  </si>
+  <si>
+    <t>Heriberto</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>0149</t>
+  </si>
+  <si>
+    <t>Angla</t>
+  </si>
+  <si>
+    <t>O'Kon</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Schmitt</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>0150</t>
+  </si>
+  <si>
+    <t>0141</t>
+  </si>
+  <si>
+    <t>herma.rodriguez</t>
+  </si>
+  <si>
+    <t>1069</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Hagenes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1078,16 +1139,16 @@
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.21875"/>
+    <col min="3" max="3" customWidth="true" width="30.33203125"/>
+    <col min="4" max="4" customWidth="true" width="62.109375"/>
+    <col min="5" max="5" customWidth="true" width="16.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1127,7 +1188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1205,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1222,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1178,7 +1239,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1195,7 +1256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1212,7 +1273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1229,7 +1290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1324,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1280,7 +1341,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1297,7 +1358,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1314,7 +1375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1331,7 +1392,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1348,7 +1409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1365,7 +1426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1382,7 +1443,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1399,7 +1460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1416,7 +1477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1433,7 +1494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1511,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1467,7 +1528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1484,7 +1545,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1579,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1535,7 +1596,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1552,7 +1613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1569,7 +1630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1586,7 +1647,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1603,7 +1664,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1620,7 +1681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1637,7 +1698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1654,7 +1715,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1671,7 +1732,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1688,7 +1749,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1705,7 +1766,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1783,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1739,7 +1800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1756,7 +1817,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +1834,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>198</v>
       </c>
@@ -1805,22 +1866,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.33203125"/>
+    <col min="2" max="2" customWidth="true" width="10.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.5546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1877,6 +1938,12 @@
       <c r="E2" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" t="s">
+        <v>227</v>
+      </c>
       <c r="H2" t="s">
         <v>73</v>
       </c>
@@ -1892,8 +1959,11 @@
       <c r="L2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1909,6 +1979,12 @@
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" t="s">
+        <v>220</v>
+      </c>
       <c r="H3" t="s">
         <v>74</v>
       </c>
@@ -1924,8 +2000,11 @@
       <c r="L3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1966,7 +2045,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1998,7 +2077,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2051,19 +2130,19 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.90625" customWidth="1"/>
-    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="8" max="8" customWidth="true" width="23.88671875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2092,7 +2171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2115,7 +2194,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2131,6 +2210,12 @@
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" t="s">
+        <v>230</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>72</v>
       </c>
@@ -2138,7 +2223,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2161,7 +2246,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2272,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2242,27 +2327,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BC94E3-296F-4311-83A2-9D6323C2EB33}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.77734375"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="3" max="3" customWidth="true" width="15.6640625"/>
+    <col min="4" max="4" customWidth="true" width="11.77734375"/>
+    <col min="5" max="6" customWidth="true" width="15.21875"/>
+    <col min="7" max="7" customWidth="true" width="13.33203125"/>
+    <col min="8" max="8" customWidth="true" width="10.88671875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6640625"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +2391,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2345,7 +2430,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2384,7 +2469,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2423,7 +2508,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2462,7 +2547,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2479,16 +2564,16 @@
         <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="G6" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="H6" t="s">
         <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
         <v>152</v>
@@ -2527,18 +2612,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.88671875"/>
+    <col min="3" max="3" customWidth="true" width="19.0"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625"/>
+    <col min="5" max="5" customWidth="true" width="12.77734375"/>
+    <col min="6" max="6" customWidth="true" width="20.88671875"/>
+    <col min="7" max="7" customWidth="true" width="16.77734375"/>
+    <col min="8" max="8" customWidth="true" width="18.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2564,7 +2649,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2590,7 +2675,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2616,7 +2701,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2642,7 +2727,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2668,7 +2753,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2711,26 +2796,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF36DA3-9270-481D-9396-013591031C0A}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="27.08984375" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.6640625"/>
+    <col min="2" max="2" customWidth="true" width="11.0"/>
+    <col min="3" max="3" customWidth="true" width="25.21875"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625"/>
+    <col min="5" max="5" customWidth="true" width="14.5546875"/>
+    <col min="6" max="6" customWidth="true" width="11.21875"/>
+    <col min="7" max="7" customWidth="true" width="10.44140625"/>
+    <col min="8" max="8" customWidth="true" width="27.109375"/>
+    <col min="9" max="9" customWidth="true" width="22.33203125"/>
+    <col min="10" max="10" customWidth="true" width="16.77734375"/>
+    <col min="11" max="11" customWidth="true" width="16.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +2850,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2791,7 +2876,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2902,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2843,7 +2928,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2869,7 +2954,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2886,13 +2971,13 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H6" t="s">
         <v>212</v>
-      </c>
-      <c r="G6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H6" t="s">
-        <v>214</v>
       </c>
       <c r="I6" t="s">
         <v>186</v>
@@ -2904,31 +2989,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -2952,16 +3037,16 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.88671875"/>
+    <col min="2" max="2" customWidth="true" width="9.77734375"/>
+    <col min="3" max="3" customWidth="true" width="17.21875"/>
+    <col min="4" max="4" customWidth="true" width="22.77734375"/>
+    <col min="5" max="5" customWidth="true" width="14.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3063,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2995,7 +3080,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3012,7 +3097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3029,7 +3114,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3046,7 +3131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3088,16 +3173,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="7.21875"/>
+    <col min="2" max="2" customWidth="true" width="12.109375"/>
+    <col min="3" max="3" customWidth="true" width="22.77734375"/>
+    <col min="4" max="4" customWidth="true" width="25.21875"/>
+    <col min="5" max="5" customWidth="true" width="16.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3114,7 +3199,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3131,7 +3216,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3148,7 +3233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3165,7 +3250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3182,7 +3267,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3224,16 +3309,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.77734375"/>
+    <col min="2" max="2" customWidth="true" width="12.0"/>
+    <col min="3" max="3" customWidth="true" width="16.109375"/>
+    <col min="4" max="4" customWidth="true" width="23.88671875"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3335,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3267,7 +3352,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3284,7 +3369,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3301,7 +3386,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3318,7 +3403,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Screenshot Code added to TC06
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F359A5C6-CC52-4F2E-848D-C9471FC3501D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2871CA5-08D7-4EF4-9733-1827C32C2673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="229">
   <si>
     <t>S. No</t>
   </si>
@@ -667,60 +667,9 @@
     <t>1079</t>
   </si>
   <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>sammie.wintheiser</t>
-  </si>
-  <si>
-    <t>Layla</t>
-  </si>
-  <si>
-    <t>Haley</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/ravi-c-1b35b1124/</t>
   </si>
   <si>
-    <t>1104</t>
-  </si>
-  <si>
-    <t>McKenzie</t>
-  </si>
-  <si>
-    <t>1132</t>
-  </si>
-  <si>
-    <t>Wiza</t>
-  </si>
-  <si>
-    <t>Jayna</t>
-  </si>
-  <si>
-    <t>Cronin</t>
-  </si>
-  <si>
-    <t>Heriberto</t>
-  </si>
-  <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>0149</t>
-  </si>
-  <si>
-    <t>Angla</t>
-  </si>
-  <si>
-    <t>O'Kon</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Schmitt</t>
-  </si>
-  <si>
     <t>Val</t>
   </si>
   <si>
@@ -730,29 +679,61 @@
     <t>0150</t>
   </si>
   <si>
-    <t>0141</t>
-  </si>
-  <si>
-    <t>herma.rodriguez</t>
-  </si>
-  <si>
-    <t>1069</t>
-  </si>
-  <si>
-    <t>Gibson</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Hagenes</t>
+    <t>1057</t>
+  </si>
+  <si>
+    <t>lesia.kiehn</t>
+  </si>
+  <si>
+    <t>Donnie</t>
+  </si>
+  <si>
+    <t>Legros</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Hills</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Greenholt</t>
+  </si>
+  <si>
+    <t>Dalton</t>
+  </si>
+  <si>
+    <t>Tillman</t>
+  </si>
+  <si>
+    <t>0151</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>reiko.bradtke</t>
+  </si>
+  <si>
+    <t>0146</t>
+  </si>
+  <si>
+    <t>Harber</t>
+  </si>
+  <si>
+    <t>1075</t>
+  </si>
+  <si>
+    <t>Leuschke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1139,16 +1120,16 @@
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.21875"/>
-    <col min="3" max="3" customWidth="true" width="30.33203125"/>
-    <col min="4" max="4" customWidth="true" width="62.109375"/>
-    <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="62.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1188,7 +1169,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1203,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1239,7 +1220,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1237,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1290,7 +1271,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1288,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1305,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1341,7 +1322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1339,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1375,7 +1356,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1392,7 +1373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1390,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1426,7 +1407,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1443,7 +1424,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1460,7 +1441,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1458,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1494,7 +1475,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1511,7 +1492,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1528,7 +1509,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1526,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1562,7 +1543,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1579,7 +1560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1596,7 +1577,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1613,7 +1594,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1630,7 +1611,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1647,7 +1628,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1664,7 +1645,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1681,7 +1662,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1679,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1696,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1732,7 +1713,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1749,7 +1730,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1766,7 +1747,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1783,7 +1764,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1800,7 +1781,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1817,7 +1798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1834,7 +1815,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>198</v>
       </c>
@@ -1866,22 +1847,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.33203125"/>
-    <col min="2" max="2" customWidth="true" width="10.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.21875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.5546875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="1" max="1" width="6.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1939,10 +1920,10 @@
         <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="G2" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="H2" t="s">
         <v>73</v>
@@ -1960,10 +1941,10 @@
         <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1980,10 +1961,10 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -2001,10 +1982,10 @@
         <v>84</v>
       </c>
       <c r="M3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2026,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2061,6 +2042,12 @@
       <c r="E5" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="F5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G5" t="s">
+        <v>215</v>
+      </c>
       <c r="H5" t="s">
         <v>76</v>
       </c>
@@ -2077,7 +2064,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2092,6 +2079,12 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" t="s">
+        <v>219</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>
@@ -2130,19 +2123,19 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.109375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5546875"/>
-    <col min="8" max="8" customWidth="true" width="23.88671875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="25.109375"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.90625" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2164,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2194,7 +2187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2211,10 +2204,10 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>72</v>
@@ -2223,7 +2216,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2246,7 +2239,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2272,7 +2265,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2289,10 +2282,10 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G6" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>72</v>
@@ -2328,26 +2321,26 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.77734375"/>
-    <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="3" max="3" customWidth="true" width="15.6640625"/>
-    <col min="4" max="4" customWidth="true" width="11.77734375"/>
-    <col min="5" max="6" customWidth="true" width="15.21875"/>
-    <col min="7" max="7" customWidth="true" width="13.33203125"/>
-    <col min="8" max="8" customWidth="true" width="10.88671875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.5546875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2384,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2430,7 +2423,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2446,12 +2439,17 @@
       <c r="E3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" t="s">
+        <v>228</v>
+      </c>
       <c r="H3" t="s">
         <v>144</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
         <v>149</v>
@@ -2469,7 +2467,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2508,7 +2506,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2547,7 +2545,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2564,10 +2562,10 @@
         <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H6" t="s">
         <v>147</v>
@@ -2612,18 +2610,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.88671875"/>
-    <col min="3" max="3" customWidth="true" width="19.0"/>
-    <col min="4" max="4" customWidth="true" width="11.6640625"/>
-    <col min="5" max="5" customWidth="true" width="12.77734375"/>
-    <col min="6" max="6" customWidth="true" width="20.88671875"/>
-    <col min="7" max="7" customWidth="true" width="16.77734375"/>
-    <col min="8" max="8" customWidth="true" width="18.5546875"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2647,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2675,7 +2673,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2701,7 +2699,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2727,7 +2725,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2753,7 +2751,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2800,22 +2798,22 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.6640625"/>
-    <col min="2" max="2" customWidth="true" width="11.0"/>
-    <col min="3" max="3" customWidth="true" width="25.21875"/>
-    <col min="4" max="4" customWidth="true" width="10.44140625"/>
-    <col min="5" max="5" customWidth="true" width="14.5546875"/>
-    <col min="6" max="6" customWidth="true" width="11.21875"/>
-    <col min="7" max="7" customWidth="true" width="10.44140625"/>
-    <col min="8" max="8" customWidth="true" width="27.109375"/>
-    <col min="9" max="9" customWidth="true" width="22.33203125"/>
-    <col min="10" max="10" customWidth="true" width="16.77734375"/>
-    <col min="11" max="11" customWidth="true" width="16.0"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="27.08984375" customWidth="1"/>
+    <col min="9" max="9" width="22.36328125" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2850,7 +2848,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +2900,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2954,7 +2952,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2971,13 +2969,13 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="H6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I6" t="s">
         <v>186</v>
@@ -2989,31 +2987,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -3037,16 +3035,16 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.88671875"/>
-    <col min="2" max="2" customWidth="true" width="9.77734375"/>
-    <col min="3" max="3" customWidth="true" width="17.21875"/>
-    <col min="4" max="4" customWidth="true" width="22.77734375"/>
-    <col min="5" max="5" customWidth="true" width="14.88671875"/>
+    <col min="1" max="1" width="5.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3063,7 +3061,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3080,7 +3078,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3097,7 +3095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3114,7 +3112,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3131,7 +3129,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3173,16 +3171,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.21875"/>
-    <col min="2" max="2" customWidth="true" width="12.109375"/>
-    <col min="3" max="3" customWidth="true" width="22.77734375"/>
-    <col min="4" max="4" customWidth="true" width="25.21875"/>
-    <col min="5" max="5" customWidth="true" width="16.6640625"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3199,7 +3197,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3216,7 +3214,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3233,7 +3231,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3250,7 +3248,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3267,7 +3265,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3306,19 +3304,19 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.77734375"/>
-    <col min="2" max="2" customWidth="true" width="12.0"/>
-    <col min="3" max="3" customWidth="true" width="16.109375"/>
-    <col min="4" max="4" customWidth="true" width="23.88671875"/>
-    <col min="5" max="5" customWidth="true" width="15.5546875"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3335,7 +3333,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3352,7 +3350,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3369,7 +3367,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3386,7 +3384,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3403,7 +3401,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Framework folder structure is reorganized
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="231">
   <si>
     <t>S. No</t>
   </si>
@@ -728,12 +728,19 @@
   </si>
   <si>
     <t>Leuschke</t>
+  </si>
+  <si>
+    <t>Loree</t>
+  </si>
+  <si>
+    <t>Hickle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,11 +1129,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.1796875"/>
+    <col min="3" max="3" customWidth="true" width="30.36328125"/>
+    <col min="4" max="4" customWidth="true" width="62.08984375"/>
+    <col min="5" max="5" customWidth="true" width="16.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1849,17 +1856,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.36328125" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.36328125"/>
+    <col min="2" max="2" customWidth="true" width="10.1796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.90625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.54296875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -2081,10 +2088,10 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="G6" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>
@@ -2125,14 +2132,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.90625" customWidth="1"/>
-    <col min="9" max="9" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.08984375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.81640625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.54296875"/>
+    <col min="8" max="8" customWidth="true" width="23.90625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.08984375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -2326,18 +2333,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.81640625"/>
+    <col min="2" max="2" customWidth="true" width="10.0"/>
+    <col min="3" max="3" customWidth="true" width="15.6328125"/>
+    <col min="4" max="4" customWidth="true" width="11.81640625"/>
+    <col min="5" max="6" customWidth="true" width="15.1796875"/>
+    <col min="7" max="7" customWidth="true" width="13.36328125"/>
+    <col min="8" max="8" customWidth="true" width="10.90625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.54296875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6328125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.90625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -2612,13 +2619,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="10.90625"/>
+    <col min="3" max="3" customWidth="true" width="19.0"/>
+    <col min="4" max="4" customWidth="true" width="11.6328125"/>
+    <col min="5" max="5" customWidth="true" width="12.81640625"/>
+    <col min="6" max="6" customWidth="true" width="20.90625"/>
+    <col min="7" max="7" customWidth="true" width="16.81640625"/>
+    <col min="8" max="8" customWidth="true" width="18.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2800,17 +2807,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="27.08984375" customWidth="1"/>
-    <col min="9" max="9" width="22.36328125" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.6328125"/>
+    <col min="2" max="2" customWidth="true" width="11.0"/>
+    <col min="3" max="3" customWidth="true" width="25.1796875"/>
+    <col min="4" max="4" customWidth="true" width="10.453125"/>
+    <col min="5" max="5" customWidth="true" width="14.54296875"/>
+    <col min="6" max="6" customWidth="true" width="11.1796875"/>
+    <col min="7" max="7" customWidth="true" width="10.453125"/>
+    <col min="8" max="8" customWidth="true" width="27.08984375"/>
+    <col min="9" max="9" customWidth="true" width="22.36328125"/>
+    <col min="10" max="10" customWidth="true" width="16.81640625"/>
+    <col min="11" max="11" customWidth="true" width="16.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -3037,11 +3044,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.90625"/>
+    <col min="2" max="2" customWidth="true" width="9.81640625"/>
+    <col min="3" max="3" customWidth="true" width="17.1796875"/>
+    <col min="4" max="4" customWidth="true" width="22.81640625"/>
+    <col min="5" max="5" customWidth="true" width="14.90625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3173,11 +3180,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="7.1796875"/>
+    <col min="2" max="2" customWidth="true" width="12.08984375"/>
+    <col min="3" max="3" customWidth="true" width="14.6328125"/>
+    <col min="4" max="4" customWidth="true" width="25.1796875"/>
+    <col min="5" max="5" customWidth="true" width="16.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3309,11 +3316,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="23.90625" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.81640625"/>
+    <col min="2" max="2" customWidth="true" width="12.0"/>
+    <col min="3" max="3" customWidth="true" width="16.08984375"/>
+    <col min="4" max="4" customWidth="true" width="23.90625"/>
+    <col min="5" max="5" customWidth="true" width="15.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
PageFactory and FindBy annotations are introduced
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="233">
   <si>
     <t>S. No</t>
   </si>
@@ -734,6 +734,12 @@
   </si>
   <si>
     <t>Hickle</t>
+  </si>
+  <si>
+    <t>Sarai</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
   </si>
 </sst>
 </file>
@@ -2088,10 +2094,10 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
pages added to demowebshop
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="235">
   <si>
     <t>S. No</t>
   </si>
@@ -740,6 +740,12 @@
   </si>
   <si>
     <t>Reynolds</t>
+  </si>
+  <si>
+    <t>Jarrett</t>
+  </si>
+  <si>
+    <t>Balistreri</t>
   </si>
 </sst>
 </file>
@@ -2094,10 +2100,10 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
framework code reorganizing into pages
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anitha\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AaradhyaVashisht\IdeaProjects\AutomationCatalogue\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2871CA5-08D7-4EF4-9733-1827C32C2673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91F96F1-188C-4CD8-99B9-80A68642F2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="722" firstSheet="2" activeTab="3" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="722" firstSheet="2" activeTab="7" xr2:uid="{32503197-61E5-4F9B-BD8F-CDA378A0F384}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="231">
   <si>
     <t>S. No</t>
   </si>
@@ -697,12 +697,6 @@
     <t>Hills</t>
   </si>
   <si>
-    <t>Gregory</t>
-  </si>
-  <si>
-    <t>Greenholt</t>
-  </si>
-  <si>
     <t>Dalton</t>
   </si>
   <si>
@@ -730,22 +724,16 @@
     <t>Leuschke</t>
   </si>
   <si>
-    <t>Loree</t>
-  </si>
-  <si>
-    <t>Hickle</t>
-  </si>
-  <si>
-    <t>Sarai</t>
-  </si>
-  <si>
-    <t>Reynolds</t>
-  </si>
-  <si>
     <t>Jarrett</t>
   </si>
   <si>
     <t>Balistreri</t>
+  </si>
+  <si>
+    <t>Order Number</t>
+  </si>
+  <si>
+    <t>Order number: 1270781</t>
   </si>
 </sst>
 </file>
@@ -1139,16 +1127,16 @@
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="12.1796875"/>
-    <col min="3" max="3" customWidth="true" width="30.36328125"/>
-    <col min="4" max="4" customWidth="true" width="62.08984375"/>
+    <col min="2" max="2" customWidth="true" width="12.21875"/>
+    <col min="3" max="3" customWidth="true" width="30.33203125"/>
+    <col min="4" max="4" customWidth="true" width="62.109375"/>
     <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.1796875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1188,7 +1176,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1239,7 +1227,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1244,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1261,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1290,7 +1278,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1295,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1312,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1341,7 +1329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1375,7 +1363,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1392,7 +1380,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1426,7 +1414,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1443,7 +1431,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1460,7 +1448,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1477,7 +1465,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1494,7 +1482,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1511,7 +1499,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1528,7 +1516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1533,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1562,7 +1550,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1579,7 +1567,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1596,7 +1584,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1613,7 +1601,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1630,7 +1618,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1647,7 +1635,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1664,7 +1652,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1681,7 +1669,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1686,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1732,7 +1720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1749,7 +1737,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1766,7 +1754,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1783,7 +1771,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1800,7 +1788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1817,7 +1805,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1834,7 +1822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>198</v>
       </c>
@@ -1866,22 +1854,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.36328125"/>
-    <col min="2" max="2" customWidth="true" width="10.1796875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.1796875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.90625"/>
+    <col min="1" max="1" customWidth="true" width="6.33203125"/>
+    <col min="2" max="2" customWidth="true" width="10.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.21875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="21.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.36328125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.54296875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.5546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1910,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1963,7 +1951,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1980,10 +1968,10 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -2001,10 +1989,10 @@
         <v>84</v>
       </c>
       <c r="M3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2033,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2071,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2100,10 +2088,10 @@
         <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G6" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H6" t="s">
         <v>77</v>
@@ -2142,19 +2130,19 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.08984375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.90625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.36328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.81640625"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.54296875"/>
-    <col min="8" max="8" customWidth="true" width="23.90625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="25.08984375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5546875"/>
+    <col min="8" max="8" customWidth="true" width="23.88671875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2206,7 +2194,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2223,10 +2211,10 @@
         <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>72</v>
@@ -2235,7 +2223,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2258,7 +2246,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2272,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2339,27 +2327,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BC94E3-296F-4311-83A2-9D6323C2EB33}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.81640625"/>
+    <col min="1" max="1" customWidth="true" width="4.77734375"/>
     <col min="2" max="2" customWidth="true" width="10.0"/>
-    <col min="3" max="3" customWidth="true" width="15.6328125"/>
-    <col min="4" max="4" customWidth="true" width="11.81640625"/>
-    <col min="5" max="6" customWidth="true" width="15.1796875"/>
-    <col min="7" max="7" customWidth="true" width="13.36328125"/>
-    <col min="8" max="8" customWidth="true" width="10.90625"/>
+    <col min="3" max="3" customWidth="true" width="15.6640625"/>
+    <col min="4" max="4" customWidth="true" width="11.77734375"/>
+    <col min="5" max="6" customWidth="true" width="15.21875"/>
+    <col min="7" max="7" customWidth="true" width="13.33203125"/>
+    <col min="8" max="8" customWidth="true" width="10.88671875"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="21.0"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="24.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.54296875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6328125"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.90625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.5546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.6640625"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2391,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2442,7 +2430,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2459,10 +2447,10 @@
         <v>72</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H3" t="s">
         <v>144</v>
@@ -2486,7 +2474,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2525,7 +2513,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2564,7 +2552,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2581,10 +2569,10 @@
         <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H6" t="s">
         <v>147</v>
@@ -2629,18 +2617,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="10.90625"/>
+    <col min="2" max="2" customWidth="true" width="10.88671875"/>
     <col min="3" max="3" customWidth="true" width="19.0"/>
-    <col min="4" max="4" customWidth="true" width="11.6328125"/>
-    <col min="5" max="5" customWidth="true" width="12.81640625"/>
-    <col min="6" max="6" customWidth="true" width="20.90625"/>
-    <col min="7" max="7" customWidth="true" width="16.81640625"/>
-    <col min="8" max="8" customWidth="true" width="18.54296875"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625"/>
+    <col min="5" max="5" customWidth="true" width="12.77734375"/>
+    <col min="6" max="6" customWidth="true" width="20.88671875"/>
+    <col min="7" max="7" customWidth="true" width="16.77734375"/>
+    <col min="8" max="8" customWidth="true" width="18.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2654,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2692,7 +2680,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2718,7 +2706,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2744,7 +2732,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2770,7 +2758,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2817,22 +2805,22 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.6328125"/>
+    <col min="1" max="1" customWidth="true" width="6.6640625"/>
     <col min="2" max="2" customWidth="true" width="11.0"/>
-    <col min="3" max="3" customWidth="true" width="25.1796875"/>
-    <col min="4" max="4" customWidth="true" width="10.453125"/>
-    <col min="5" max="5" customWidth="true" width="14.54296875"/>
-    <col min="6" max="6" customWidth="true" width="11.1796875"/>
-    <col min="7" max="7" customWidth="true" width="10.453125"/>
-    <col min="8" max="8" customWidth="true" width="27.08984375"/>
-    <col min="9" max="9" customWidth="true" width="22.36328125"/>
-    <col min="10" max="10" customWidth="true" width="16.81640625"/>
+    <col min="3" max="3" customWidth="true" width="25.21875"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625"/>
+    <col min="5" max="5" customWidth="true" width="14.5546875"/>
+    <col min="6" max="6" customWidth="true" width="11.21875"/>
+    <col min="7" max="7" customWidth="true" width="10.44140625"/>
+    <col min="8" max="8" customWidth="true" width="27.109375"/>
+    <col min="9" max="9" customWidth="true" width="22.33203125"/>
+    <col min="10" max="10" customWidth="true" width="16.77734375"/>
     <col min="11" max="11" customWidth="true" width="16.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +2855,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2893,7 +2881,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2919,7 +2907,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2945,7 +2933,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +2959,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3006,31 +2994,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
   </sheetData>
@@ -3048,22 +3036,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1433F4D-AA94-4C23-B8F4-C641A3F219D9}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F1" sqref="F1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.90625"/>
-    <col min="2" max="2" customWidth="true" width="9.81640625"/>
-    <col min="3" max="3" customWidth="true" width="17.1796875"/>
-    <col min="4" max="4" customWidth="true" width="22.81640625"/>
-    <col min="5" max="5" customWidth="true" width="14.90625"/>
+    <col min="1" max="1" customWidth="true" width="5.88671875"/>
+    <col min="2" max="2" customWidth="true" width="9.77734375"/>
+    <col min="3" max="3" customWidth="true" width="17.21875"/>
+    <col min="4" max="4" customWidth="true" width="22.77734375"/>
+    <col min="5" max="5" customWidth="true" width="14.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3079,8 +3068,11 @@
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3097,7 +3089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3114,7 +3106,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3131,7 +3123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3148,7 +3140,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3163,6 +3155,9 @@
       </c>
       <c r="E6" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3184,22 +3179,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A32D993-D624-4A5F-A345-C2B190736A2C}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.1796875"/>
-    <col min="2" max="2" customWidth="true" width="12.08984375"/>
-    <col min="3" max="3" customWidth="true" width="14.6328125"/>
-    <col min="4" max="4" customWidth="true" width="25.1796875"/>
-    <col min="5" max="5" customWidth="true" width="16.6328125"/>
+    <col min="1" max="1" customWidth="true" width="7.21875"/>
+    <col min="2" max="2" customWidth="true" width="12.109375"/>
+    <col min="3" max="3" customWidth="true" width="14.6640625"/>
+    <col min="4" max="4" customWidth="true" width="25.21875"/>
+    <col min="5" max="5" customWidth="true" width="16.6640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3215,8 +3211,11 @@
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3326,16 +3325,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="5.81640625"/>
+    <col min="1" max="1" customWidth="true" width="5.77734375"/>
     <col min="2" max="2" customWidth="true" width="12.0"/>
-    <col min="3" max="3" customWidth="true" width="16.08984375"/>
-    <col min="4" max="4" customWidth="true" width="23.90625"/>
-    <col min="5" max="5" customWidth="true" width="15.54296875"/>
+    <col min="3" max="3" customWidth="true" width="16.109375"/>
+    <col min="4" max="4" customWidth="true" width="23.88671875"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3386,7 +3385,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3420,7 +3419,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>